<commit_message>
Updated SWGCalculator.xlsx, README.md, and .gitignore
Create .gitignore and ignoring temp excel files.
Updated README.md with correct excel ranges.
SWGCalculator.xlsx:
    Update instructions
    Add description of colored ranges
    Renamed "Min Runtime" to "Max Acceptable" and Max Runtime to Max Possible (24)
    Added setting for SWG % increments, only effects "Calculate SWG %" in bottom left
</commit_message>
<xml_diff>
--- a/SWGCalculator.xlsx
+++ b/SWGCalculator.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="22650" yWindow="0" windowWidth="3615" windowHeight="8505"/>
@@ -12,8 +12,9 @@
     <sheet name="Setup" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Max_Runtime">Runtime[Max Runtime]</definedName>
-    <definedName name="Min_Runtime">Runtime[Min Runtime]</definedName>
+    <definedName name="Max_Runtime">Runtime[Max possible (24)]</definedName>
+    <definedName name="Min_Runtime">Runtime[Max acceptable]</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Calculator!$B$1:$M$28</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
   <si>
     <t>FC</t>
   </si>
@@ -132,24 +133,9 @@
     <t>Instructions:</t>
   </si>
   <si>
-    <t>1. Enter your Pool Volume in gallons in cell D4</t>
-  </si>
-  <si>
-    <t>2. Enter your Average 24 Hr FC Demand in cell D5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Enter the production of your SWG in lbs in cell D6.  See link for this value.  </t>
-  </si>
-  <si>
-    <t>4. Enter a SWG Output % in cell D10.  Use this % and the Hours output to set your SWG &amp; Pump Run Time.</t>
-  </si>
-  <si>
     <t>or</t>
   </si>
   <si>
-    <t>4. Enter a Desired Run Time in cell D16.  Use these hours and the Output % to set your SWG &amp; Pump Run Time.</t>
-  </si>
-  <si>
     <t>4. Use the SWG Run Time Chart to determine the Output % &amp; Pump Run Time based on the FC PPM Demand</t>
   </si>
   <si>
@@ -180,12 +166,6 @@
     <t>Updated header / footer and print settings</t>
   </si>
   <si>
-    <t>Min Runtime</t>
-  </si>
-  <si>
-    <t>Max Runtime</t>
-  </si>
-  <si>
     <t>Beta 1.3</t>
   </si>
   <si>
@@ -202,6 +182,72 @@
   </si>
   <si>
     <t>Modified by Lightmaster</t>
+  </si>
+  <si>
+    <t>1. Enter your Pool Volume in gallons in cell D6</t>
+  </si>
+  <si>
+    <t>2. Enter your Average 24 Hr FC Demand in cell D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Enter the production of your SWG in lbs in cell D8.  See link for this value.  </t>
+  </si>
+  <si>
+    <t>4. Enter a SWG Output % in cell D14.  Use this % and the Hours output to set your SWG &amp; Pump Run Time.</t>
+  </si>
+  <si>
+    <t>4. Enter a Desired Run Time in cell D23.  Use these hours and the Output % to set your SWG &amp; Pump Run Time.</t>
+  </si>
+  <si>
+    <t>Green: Acceptable</t>
+  </si>
+  <si>
+    <t>Yellow: Possible, but exceeds acceptable</t>
+  </si>
+  <si>
+    <t>Red: Physically impossible</t>
+  </si>
+  <si>
+    <t>Beta 1.4</t>
+  </si>
+  <si>
+    <t>Update instructions</t>
+  </si>
+  <si>
+    <t>Add description of colored ranges</t>
+  </si>
+  <si>
+    <t>Max acceptable</t>
+  </si>
+  <si>
+    <t>Max possible (24)</t>
+  </si>
+  <si>
+    <t>(Green)</t>
+  </si>
+  <si>
+    <t>(Red)</t>
+  </si>
+  <si>
+    <t>Max Acceptable (Green): Enter the highest runtime you'd consider to be acceptable. IE: 10 means you want all hours below 10 to be acceptable</t>
+  </si>
+  <si>
+    <t>Max Possible (Red): Maximum physically possible time to be able to run your pump in a 24 hour period. IE: 24 since you can't physically run it more than 24 hours in a day.</t>
+  </si>
+  <si>
+    <t>Renamed "Min Runtime" to "Max Acceptable" and Max Runtime to Max Possible (24)</t>
+  </si>
+  <si>
+    <t>"SWG % Calculator"</t>
+  </si>
+  <si>
+    <t>SWG % increments for</t>
+  </si>
+  <si>
+    <t>SWG % increments: Set this to whatever percentage increments your SWG allows. Most allow adjustment by 5% increments, although some allow 1% and some only 10%.</t>
+  </si>
+  <si>
+    <t>Added setting for SWG % increments, only effects "Calculate SWG %" in bottom left</t>
   </si>
 </sst>
 </file>
@@ -217,7 +263,7 @@
     <numFmt numFmtId="168" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="169" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,8 +362,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,6 +419,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBDD7EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -619,7 +699,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -791,6 +871,46 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -798,10 +918,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <numFmt numFmtId="168" formatCode="mm/dd/yyyy"/>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -833,6 +950,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFFF0000"/>
@@ -851,10 +974,19 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="mm/dd/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -875,11 +1007,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="$D$14" horiz="1" inc="5" max="100" page="10" val="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="$D$14" horiz="1" inc="5" max="100" page="10" val="15"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="$D$23" horiz="1" max="24" page="2" val="8"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="16" fmlaLink="$D$23" horiz="1" max="24" page="2" val="4"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -970,11 +1102,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C15" totalsRowShown="0">
-  <autoFilter ref="A1:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C19" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Version"/>
-    <tableColumn id="3" name="Date" dataDxfId="0"/>
+    <tableColumn id="3" name="Date" dataDxfId="9"/>
     <tableColumn id="2" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -982,10 +1113,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Runtime" displayName="Runtime" ref="A1:B2" totalsRowShown="0">
-  <tableColumns count="2">
-    <tableColumn id="1" name="Min Runtime"/>
-    <tableColumn id="2" name="Max Runtime"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Runtime" displayName="Runtime" ref="A1:C3" totalsRowShown="0" dataDxfId="6">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Max acceptable" dataDxfId="8"/>
+    <tableColumn id="2" name="Max possible (24)" dataDxfId="7"/>
+    <tableColumn id="3" name="SWG % increments for" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1280,7 +1412,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1289,10 +1421,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:M42"/>
+  <dimension ref="B1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,9 +1439,9 @@
     <col min="9" max="13" width="7.7109375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" ht="23.25" x14ac:dyDescent="0.3">
       <c r="B1" s="24" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -1322,16 +1454,16 @@
       <c r="K1" s="24"/>
       <c r="L1" s="24"/>
       <c r="M1" s="25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="2:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="37" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C2" s="37"/>
       <c r="D2" s="37" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="37"/>
@@ -1345,10 +1477,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="21" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" ht="21" x14ac:dyDescent="0.3">
       <c r="B4" s="27"/>
       <c r="C4" s="77" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D4" s="77"/>
       <c r="E4" s="77"/>
@@ -1362,7 +1494,7 @@
       <c r="L4" s="57"/>
       <c r="M4" s="57"/>
     </row>
-    <row r="5" spans="2:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="29"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1376,7 +1508,7 @@
       <c r="L5" s="16"/>
       <c r="M5" s="17"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="29"/>
       <c r="C6" s="9" t="s">
         <v>3</v>
@@ -1400,7 +1532,7 @@
       <c r="L6" s="59"/>
       <c r="M6" s="60"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="29"/>
       <c r="C7" s="9" t="s">
         <v>13</v>
@@ -1432,7 +1564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="29"/>
       <c r="C8" s="11" t="s">
         <v>11</v>
@@ -1468,8 +1600,14 @@
         <f t="shared" si="0"/>
         <v>67.099999999999994</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="84" t="s">
+        <v>57</v>
+      </c>
+      <c r="O8" s="83"/>
+      <c r="P8" s="83"/>
+      <c r="Q8" s="83"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="29"/>
       <c r="C9" s="9" t="s">
         <v>10</v>
@@ -1506,8 +1644,14 @@
         <f t="shared" si="1"/>
         <v>33.5</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="84" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" s="83"/>
+      <c r="P9" s="83"/>
+      <c r="Q9" s="83"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="31"/>
       <c r="C10" s="32" t="s">
         <v>2</v>
@@ -1544,8 +1688,14 @@
         <f t="shared" si="1"/>
         <v>22.4</v>
       </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="84" t="s">
+        <v>59</v>
+      </c>
+      <c r="O10" s="83"/>
+      <c r="P10" s="83"/>
+      <c r="Q10" s="83"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="F11" s="35"/>
       <c r="G11" s="26"/>
       <c r="H11" s="13">
@@ -1572,10 +1722,10 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" s="40"/>
       <c r="C12" s="64" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D12" s="64"/>
       <c r="E12" s="64"/>
@@ -1605,7 +1755,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="29"/>
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
@@ -1636,13 +1786,13 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" s="29"/>
       <c r="C14" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="48">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>12</v>
@@ -1673,7 +1823,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="29"/>
       <c r="C15" s="2"/>
       <c r="D15" s="5"/>
@@ -1704,11 +1854,11 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="29"/>
       <c r="C16" s="61" t="str">
         <f>"Run time to replace " &amp; D7 &amp; " PPM @ " &amp; D14 &amp; "% output"</f>
-        <v>Run time to replace 1 PPM @ 10% output</v>
+        <v>Run time to replace 1 PPM @ 15% output</v>
       </c>
       <c r="D16" s="62"/>
       <c r="E16" s="63"/>
@@ -1741,8 +1891,8 @@
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="29"/>
       <c r="C17" s="65">
-        <f>ROUND((D7/D10)/D14*100,1)</f>
-        <v>6.7</v>
+        <f>IFERROR(ROUND((D7/D10)/D14*100,1),"Enter an output greater than 0%")</f>
+        <v>4.5</v>
       </c>
       <c r="D17" s="66"/>
       <c r="E17" s="67"/>
@@ -1861,7 +2011,7 @@
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="42"/>
       <c r="C21" s="55" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D21" s="55"/>
       <c r="E21" s="55"/>
@@ -1926,7 +2076,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="49">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>20</v>
@@ -1990,7 +2140,7 @@
       <c r="B25" s="1"/>
       <c r="C25" s="61" t="str">
         <f>"Required output % to replace " &amp; D7 &amp; " PPM in " &amp; D23 &amp; " hours"</f>
-        <v>Required output % to replace 1 PPM in 8 hours</v>
+        <v>Required output % to replace 1 PPM in 4 hours</v>
       </c>
       <c r="D25" s="62"/>
       <c r="E25" s="63"/>
@@ -2022,8 +2172,8 @@
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="71">
-        <f>CEILING(D7/(D23*D10),0.05)</f>
-        <v>0.1</v>
+        <f>CEILING(D7/(D23*D10),Setup!$C$3)</f>
+        <v>0.2</v>
       </c>
       <c r="D26" s="72"/>
       <c r="E26" s="73"/>
@@ -2097,77 +2247,188 @@
       <c r="L28" s="53"/>
       <c r="M28" s="54"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="23" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D30" s="22"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B31" s="39" t="s">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="39"/>
+      <c r="C31" s="90"/>
       <c r="D31" s="39"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B32" s="39" t="s">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="39"/>
+      <c r="C32" s="90"/>
       <c r="D32" s="39"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="91"/>
       <c r="D33" s="22"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C34" s="23" t="s">
+    <row r="34" spans="2:13" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="92"/>
+      <c r="C34" s="92"/>
+      <c r="D34" s="22"/>
+    </row>
+    <row r="35" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="78" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
+      <c r="M35" s="80"/>
+    </row>
+    <row r="36" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="81" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="81"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="81"/>
+      <c r="G36" s="81"/>
+      <c r="H36" s="81"/>
+      <c r="I36" s="81"/>
+      <c r="J36" s="81"/>
+      <c r="K36" s="81"/>
+      <c r="L36" s="81"/>
+      <c r="M36" s="81"/>
+    </row>
+    <row r="37" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="81"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="81"/>
+      <c r="G37" s="81"/>
+      <c r="H37" s="81"/>
+      <c r="I37" s="81"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="81"/>
+      <c r="L37" s="81"/>
+      <c r="M37" s="81"/>
+    </row>
+    <row r="38" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="81"/>
+      <c r="E38" s="81"/>
+      <c r="F38" s="81"/>
+      <c r="G38" s="81"/>
+      <c r="H38" s="81"/>
+      <c r="I38" s="81"/>
+      <c r="J38" s="81"/>
+      <c r="K38" s="81"/>
+      <c r="L38" s="81"/>
+      <c r="M38" s="81"/>
+    </row>
+    <row r="39" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="81"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="81"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="81"/>
+      <c r="J39" s="81"/>
+      <c r="K39" s="81"/>
+      <c r="L39" s="81"/>
+      <c r="M39" s="81"/>
+    </row>
+    <row r="40" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="79" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
+      <c r="D40" s="79"/>
+      <c r="E40" s="79"/>
+      <c r="F40" s="79"/>
+      <c r="G40" s="79"/>
+      <c r="H40" s="80"/>
+      <c r="I40" s="80"/>
+      <c r="J40" s="80"/>
+      <c r="K40" s="80"/>
+      <c r="L40" s="80"/>
+      <c r="M40" s="80"/>
+    </row>
+    <row r="41" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="81" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="81"/>
+      <c r="G41" s="81"/>
+      <c r="H41" s="81"/>
+      <c r="I41" s="81"/>
+      <c r="J41" s="81"/>
+      <c r="K41" s="81"/>
+      <c r="L41" s="81"/>
+      <c r="M41" s="81"/>
+    </row>
+    <row r="42" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="79" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="79"/>
+      <c r="E42" s="79"/>
+      <c r="F42" s="79"/>
+      <c r="G42" s="79"/>
+      <c r="H42" s="80"/>
+      <c r="I42" s="80"/>
+      <c r="J42" s="80"/>
+      <c r="K42" s="80"/>
+      <c r="L42" s="80"/>
+      <c r="M42" s="80"/>
+    </row>
+    <row r="43" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="81" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>41</v>
-      </c>
+      <c r="D43" s="81"/>
+      <c r="E43" s="81"/>
+      <c r="F43" s="81"/>
+      <c r="G43" s="81"/>
+      <c r="H43" s="81"/>
+      <c r="I43" s="81"/>
+      <c r="J43" s="81"/>
+      <c r="K43" s="81"/>
+      <c r="L43" s="81"/>
+      <c r="M43" s="81"/>
     </row>
   </sheetData>
-  <sheetProtection password="F340" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="10">
+  <sheetProtection password="ECDE" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="22">
+    <mergeCell ref="C43:M43"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="C36:M36"/>
+    <mergeCell ref="C37:M37"/>
+    <mergeCell ref="C38:M38"/>
+    <mergeCell ref="C39:M39"/>
+    <mergeCell ref="C41:M41"/>
     <mergeCell ref="H28:M28"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="H4:M4"/>
@@ -2180,11 +2441,11 @@
     <mergeCell ref="C16:E16"/>
   </mergeCells>
   <conditionalFormatting sqref="I8:M27">
-    <cfRule type="expression" dxfId="5" priority="2">
-      <formula>I$7=$D$7</formula>
-    </cfRule>
     <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND($H8=$D$14/100,I$7=$D$7)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>I$7=$D$7</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -2194,20 +2455,19 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1"/>
-    <hyperlink ref="C32:D32" r:id="rId2" display="Chlorine / CYA Chart"/>
-    <hyperlink ref="C31:D31" r:id="rId3" display="Water Balance for SWGs"/>
-    <hyperlink ref="M2" r:id="rId4"/>
+    <hyperlink ref="M2" r:id="rId2"/>
+    <hyperlink ref="B33" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
-  <legacyDrawing r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId8" name="Scroll Bar 1">
+            <control shapeId="1025" r:id="rId7" name="Scroll Bar 1">
               <controlPr defaultSize="0" print="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2229,7 +2489,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId9" name="Scroll Bar 2">
+            <control shapeId="1026" r:id="rId8" name="Scroll Bar 2">
               <controlPr defaultSize="0" print="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2257,7 +2517,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="8" operator="greaterThanOrEqual" id="{F1A9E657-D870-454E-93EA-A2DEFB150498}">
-            <xm:f>Setup!$B$2</xm:f>
+            <xm:f>Setup!$B$3</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2270,7 +2530,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="9" operator="greaterThan" id="{DACBD46E-4419-4E7D-A4B9-B3C646CC984A}">
-            <xm:f>Setup!$A$2</xm:f>
+            <xm:f>Setup!$A$3</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C6500"/>
@@ -2283,7 +2543,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="10" operator="lessThanOrEqual" id="{26F9F61F-85B1-4C05-B967-9A76B675B3E9}">
-            <xm:f>Setup!$A$2</xm:f>
+            <xm:f>Setup!$A$3</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF006100"/>
@@ -2301,13 +2561,13 @@
           <x14:cfRule type="colorScale" priority="3" id="{6DA838B8-46D3-4AAD-A1DE-A01C3B0EED66}">
             <x14:colorScale>
               <x14:cfvo type="formula">
-                <xm:f>Setup!$A$2</xm:f>
+                <xm:f>Setup!$A$3</xm:f>
               </x14:cfvo>
               <x14:cfvo type="percentile">
                 <xm:f>50</xm:f>
               </x14:cfvo>
               <x14:cfvo type="formula">
-                <xm:f>Setup!$B$2</xm:f>
+                <xm:f>Setup!$B$3</xm:f>
               </x14:cfvo>
               <x14:color rgb="FF63BE7B"/>
               <x14:color rgb="FFFFEB84"/>
@@ -2325,10 +2585,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2433,7 +2693,7 @@
         <v>42604</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2444,7 +2704,7 @@
         <v>42604</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2455,40 +2715,69 @@
         <v>42604</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B12" s="50">
         <v>43153</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="50"/>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="50"/>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="50"/>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="50">
+        <v>43178</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="50"/>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="50"/>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="50"/>
+      <c r="C19" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="F340" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="ECDE" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2499,38 +2788,69 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="88" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="86" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="89" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="82">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="82">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
+      <c r="C3" s="87">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="51" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
+  <sheetProtection password="ECDE" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>